<commit_message>
Report - kapitola 4 problémy při realizaci
</commit_message>
<xml_diff>
--- a/trunk/zaverecka/FMEAt.xlsx
+++ b/trunk/zaverecka/FMEAt.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="150" windowWidth="20115" windowHeight="12075"/>
@@ -11,12 +11,12 @@
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Neudělení zápočtu</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Špatný návrh komunikačního protokolu</t>
   </si>
   <si>
-    <t>Vyčerpání možností free licence vývojového programu (&lt;32 kB)</t>
-  </si>
-  <si>
     <t>Zranění klíčového člena týmu</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>Nepochopení požadavků zadavatele</t>
   </si>
   <si>
-    <t>FMEA(T)</t>
-  </si>
-  <si>
     <t>P - pravděpodobnost   Z - závažnost   D - detekovatelnost</t>
   </si>
   <si>
@@ -123,14 +117,17 @@
     <t>Možná demotivace členů týmu</t>
   </si>
   <si>
-    <t>Ponechat rezervy ve schválených specifikacích vůči výsledkům, jeź jsme schopni dosáhnout</t>
+    <t>Vyčerpání možností free licence vývojového programu</t>
+  </si>
+  <si>
+    <t>Ponechat rezervy ve schválených specifikacích vůči výsledkům, jež jsme schopni dosáhnout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,15 +154,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -308,25 +329,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -339,7 +522,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -413,7 +596,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -448,7 +630,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kancelář">
@@ -624,289 +805,287 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="56.5703125" customWidth="1"/>
-    <col min="2" max="3" width="2.85546875" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="82.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:8" ht="22.5" customHeight="1" thickBot="1">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="24" customHeight="1">
+      <c r="B2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="2:8" ht="36" customHeight="1">
+      <c r="B3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <f>C3*D3*E3</f>
+        <v>20</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="36" customHeight="1">
+      <c r="B4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F12" si="0">C4*D4*E4</f>
+        <v>175</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="5" spans="2:8" ht="36" customHeight="1">
+      <c r="B5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D5" s="2">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <f>B3*C3*D3</f>
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" ref="E4:E12" si="0">B4*C4*D4</f>
-        <v>175</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>16</v>
+      <c r="G5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="2:8" ht="36" customHeight="1">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="4">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>17</v>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="2:8" ht="36" customHeight="1">
+      <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="4">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>7</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>10</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
+      <c r="G7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="2:8" ht="36" customHeight="1">
+      <c r="B8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>7</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>18</v>
+      <c r="G8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="9" spans="2:8" ht="36" customHeight="1">
+      <c r="B9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>9</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>16</v>
+      <c r="G9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="10" spans="2:8" ht="36" customHeight="1">
+      <c r="B10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
         <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>10</v>
       </c>
       <c r="D10" s="2">
         <v>10</v>
       </c>
       <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>19</v>
+      <c r="G10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="11" spans="2:8" ht="36" customHeight="1">
+      <c r="B11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>5</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="36" customHeight="1" thickBot="1">
+      <c r="B12" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="C12" s="6">
         <v>8</v>
       </c>
-      <c r="C12" s="9">
+      <c r="D12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="9">
+      <c r="E12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="9">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>21</v>
+      <c r="G12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -916,24 +1095,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>